<commit_message>
New version. Car + Avatar in output
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -142,10 +142,10 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -428,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,13 +953,13 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -988,7 +988,9 @@
       <c r="D28" s="10">
         <v>0.5</v>
       </c>
-      <c r="E28" s="10"/>
+      <c r="E28" s="11">
+        <v>1.1000000000000001</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1042,22 +1044,22 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="13">
+      <c r="B33" s="12">
         <v>1</v>
       </c>
-      <c r="C33" s="13">
+      <c r="C33" s="12">
         <v>2</v>
       </c>
-      <c r="D33" s="13">
+      <c r="D33" s="12">
         <v>3</v>
       </c>
       <c r="E33" t="s">

</xml_diff>